<commit_message>
Grado 11 - guion 1 Finalizado
Edición finalizada del manuscrito, de los recursos, mapa conceptual y
guía, así como envíos de solicitud gráfica. Hoy material completo
enviado a corrección de estilo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/esqueletoGuion - CS_11_01_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion01/esqueletoGuion - CS_11_01_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
     <sheet name="Hoja1" sheetId="17" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
     <author>Flor Buitrago</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="A23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,22 +57,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Yo propongo:
-Reconocer los conflictos del mundo actual nos ayuda a reflexionar acerca de la forma en que propondremos soluciones creativas y pacíficas en nuestro entorno</t>
+este es de mi autoría, revisarlo. Si quedó bien, se lo envío al autor para que haga algo parecido en la siguiente entrega</t>
         </r>
       </text>
     </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Flor Buitrago</author>
-  </authors>
-  <commentList>
-    <comment ref="B171" authorId="0" shapeId="0">
+    <comment ref="A24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,10 +81,78 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-De esta parte, el autor no entregó nada. Pendiente entonces por encargar.</t>
+No sé por qué el autor se enredó con FreeMind y no hizo el mapa conceptual en el programa indicado, lo entregó en jpg</t>
         </r>
       </text>
     </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Flor Buitrago</author>
+  </authors>
+  <commentList>
+    <comment ref="B27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Flor Buitrago:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+este es de mi autoría, revisarlo. Si quedó bien, se lo envío al autor para que haga algo parecido en la siguiente entrega</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Flor Buitrago:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No sé por qué el autor se enredó con FreeMind y no hizo el mapa conceptual en el programa indicado, lo entregó en jpg</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Flor Buitrago</author>
+  </authors>
+  <commentList>
     <comment ref="H171" authorId="0" shapeId="0">
       <text>
         <r>
@@ -120,12 +177,94 @@
         </r>
       </text>
     </comment>
+    <comment ref="H172" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Flor Buitrago:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No sé por qué el autor se enredó con FreeMind y no hizo el mapa conceptual en el programa indicado, lo entregó en jpg</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Flor Buitrago</author>
+  </authors>
+  <commentList>
+    <comment ref="A25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Flor Buitrago:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+este es de mi autoría, revisarlo. Si quedó bien, se lo envío al autor para que haga algo parecido en la siguiente entrega</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Flor Buitrago:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No sé por qué el autor se enredó con FreeMind y no hizo el mapa conceptual en el programa indicado, lo entregó en jpg</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="109">
   <si>
     <t>FICHA</t>
   </si>
@@ -229,9 +368,6 @@
     <t>Claves para comprender los conflictos del siglo XXI</t>
   </si>
   <si>
-    <t>REC10. Título pendiente, en cambio por autor</t>
-  </si>
-  <si>
     <t>REC20. El juego geopolítico global</t>
   </si>
   <si>
@@ -283,9 +419,6 @@
     <t>REC80. Formas no violentas para la resolución de conflictos</t>
   </si>
   <si>
-    <t>REC90. Nuevo. Motores de los conflictos. En elaboración por autor</t>
-  </si>
-  <si>
     <t>Conflictos bélicos actuales en Eurasia</t>
   </si>
   <si>
@@ -298,15 +431,9 @@
     <t>REC110. Comprende los nacionalismos en la Europa de hoy</t>
   </si>
   <si>
-    <t>REC120. La Unión Europea en el contexto de la crisis. Ajustes autor</t>
-  </si>
-  <si>
     <t>Rusia: el posicionamiento de un gigante y sus tensiones con la OTAN</t>
   </si>
   <si>
-    <t>REC130. Las características del neofascismo. En ajustes Autor</t>
-  </si>
-  <si>
     <t>REC140. Comprende los conflictos actuales entre Rusia y la OTAN</t>
   </si>
   <si>
@@ -328,9 +455,6 @@
     <t>Chiitas y sunitas: claves para comprender los conflictos en Medio Oriente</t>
   </si>
   <si>
-    <t>REC160. El mundo islámico. En ajustes autor</t>
-  </si>
-  <si>
     <t>Chiitas</t>
   </si>
   <si>
@@ -352,9 +476,6 @@
     <t>REC190. Analiza el movimiento social conocido como la "Primavera árabe"</t>
   </si>
   <si>
-    <t>REC200. La "Primavera árabe". En ajustes autor</t>
-  </si>
-  <si>
     <t>El programa nuclear iraní</t>
   </si>
   <si>
@@ -382,56 +503,101 @@
     <t>Evaluación II</t>
   </si>
   <si>
-    <t>REC240. Mapa Conceptual. En ajustes por el Autor</t>
-  </si>
-  <si>
-    <t>REC250. Evaluación I</t>
-  </si>
-  <si>
-    <t>REC260. Evaluación II</t>
-  </si>
-  <si>
     <t>CS_11_01_CO</t>
   </si>
   <si>
-    <t>El autor no la ha enviado</t>
-  </si>
-  <si>
     <t>Educación Básica Secundaria</t>
   </si>
   <si>
     <t>Ciencias Sociales</t>
   </si>
   <si>
-    <t>XREC270-Se titulará: Refuerza tu aprendizaje</t>
-  </si>
-  <si>
-    <t>XREC280 -Competencias…</t>
-  </si>
-  <si>
-    <t>XREC290-Competencias…</t>
-  </si>
-  <si>
     <t>REC260 Conoce tus competencias para comprender conflictos globales II</t>
   </si>
   <si>
     <t>REC250 Conoce tus competencias para comprender conflictos globales I</t>
   </si>
   <si>
-    <t>RECxx. Evaluación I</t>
-  </si>
-  <si>
-    <t>RECxx. Evaluación II</t>
-  </si>
-  <si>
     <t>REC270 Proyecto</t>
+  </si>
+  <si>
+    <t>REC10. Observa los múltiples niveles de análisis de un conflicto</t>
+  </si>
+  <si>
+    <t>REC120. Explora la crisis económica europea mediante el caso griego</t>
+  </si>
+  <si>
+    <t>REC160. El mundo islámico: entre la tradición y el cambio</t>
+  </si>
+  <si>
+    <t>REC90. Los múltiples motores de los conflictos</t>
+  </si>
+  <si>
+    <t>REC130. Conoce expresiones de xenofobia y racismo en la Europa actual</t>
+  </si>
+  <si>
+    <t>REC200. La Primavera árabe</t>
+  </si>
+  <si>
+    <t>REC280. Evaluación I</t>
+  </si>
+  <si>
+    <t>REC290. Evaluación II</t>
+  </si>
+  <si>
+    <t>Eso 4/ Ciencias Sociales/ el mundo actual/ Las potencias emergentes: Brasil, Rusia, India y China</t>
+  </si>
+  <si>
+    <t>ESO 4</t>
+  </si>
+  <si>
+    <t>El mundo actual</t>
+  </si>
+  <si>
+    <t>Las potencias emergentes: Brasil, Rusia, India y China</t>
+  </si>
+  <si>
+    <t>Eso 4/ Ciencias Sociales/El mundo actual / Los conflictos recientes/</t>
+  </si>
+  <si>
+    <t>Los conflictos recientes</t>
+  </si>
+  <si>
+    <t>El mundo islámico: entre la tradición y el cambio</t>
+  </si>
+  <si>
+    <t>Eso 4/Ciencias Sociales/El mundo actual/El mundo islámico: entre la tradición y el cambio</t>
+  </si>
+  <si>
+    <t>Este recursos requiere ajustes de imágenes</t>
+  </si>
+  <si>
+    <t>Eso 3/ Ciencias Sociales/El mundo actual: cambios y contrastes / La Primavera Árábe/</t>
+  </si>
+  <si>
+    <t>El mundo actual: cambios y contrastes</t>
+  </si>
+  <si>
+    <t>La Primavera árabe</t>
+  </si>
+  <si>
+    <t>REC210 Contextualiza la información sobre Irán y su programa nuclear</t>
+  </si>
+  <si>
+    <t>REC220 Plantea hipótesis en torno al conflicto palestino-israelí</t>
+  </si>
+  <si>
+    <t>REC 230 El uso del velo islámico</t>
+  </si>
+  <si>
+    <t>Una mirada panorámica a los conflictos globales escenificados en Europa y en Asia, identificando sus actores, los elementos y relaciones que implican desde la geopolítica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,8 +663,20 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -519,13 +697,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -955,7 +1127,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -966,9 +1138,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -990,16 +1159,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="401">
@@ -1680,11 +1853,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1867,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
@@ -1702,31 +1875,31 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>89</v>
+      <c r="B3" s="21" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1">
@@ -1734,17 +1907,16 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1758,7 +1930,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,32 +1946,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -1807,21 +1991,95 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E8" s="8"/>
+    </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G9" s="10"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="8"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G10" s="10"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G11" s="10"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G12" s="10"/>
+      <c r="G12" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1831,49 +2089,304 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
+      <c r="A2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-    </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:C65">
@@ -1881,6 +2394,7 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1890,36 +2404,352 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="6"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:C38">
@@ -1928,6 +2758,7 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="71" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -1940,9 +2771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H173" sqref="H173"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,31 +2790,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1991,442 +2822,442 @@
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="C2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="C6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="E7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="E9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="E12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>40</v>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="E14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="E16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="E19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="E21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="7"/>
+      <c r="D22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="E23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -2437,27 +3268,27 @@
       <c r="A27" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H27" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -2471,7 +3302,7 @@
       <c r="A29" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -2488,7 +3319,7 @@
       <c r="A30" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -2505,7 +3336,7 @@
       <c r="A31" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2522,7 +3353,7 @@
       <c r="A32" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2539,7 +3370,7 @@
       <c r="A33" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -2556,7 +3387,7 @@
       <c r="A34" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -2573,7 +3404,7 @@
       <c r="A35" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -2590,7 +3421,7 @@
       <c r="A36" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -2607,7 +3438,7 @@
       <c r="A37" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -2624,7 +3455,7 @@
       <c r="A38" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -2641,7 +3472,7 @@
       <c r="A39" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2658,7 +3489,7 @@
       <c r="A40" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -2671,17 +3502,17 @@
         <v>28</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D41" s="3" t="s">
@@ -2694,10 +3525,10 @@
         <v>26</v>
       </c>
       <c r="H41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I41" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2722,10 +3553,10 @@
         <v>28</v>
       </c>
       <c r="H43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2736,7 +3567,7 @@
         <v>33</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>21</v>
@@ -2750,7 +3581,7 @@
         <v>33</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>25</v>
@@ -2764,7 +3595,7 @@
         <v>33</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>21</v>
@@ -2778,7 +3609,7 @@
         <v>33</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>24</v>
@@ -2792,7 +3623,7 @@
         <v>33</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>21</v>
@@ -2806,7 +3637,7 @@
         <v>33</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>22</v>
@@ -2820,7 +3651,7 @@
         <v>33</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>21</v>
@@ -2834,16 +3665,16 @@
         <v>33</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H51" t="s">
-        <v>50</v>
-      </c>
-      <c r="I51" s="9" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2854,7 +3685,7 @@
         <v>33</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>21</v>
@@ -2868,7 +3699,7 @@
         <v>33</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>22</v>
@@ -2882,7 +3713,7 @@
         <v>33</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>21</v>
@@ -2896,7 +3727,7 @@
         <v>33</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>25</v>
@@ -2910,7 +3741,7 @@
         <v>33</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>21</v>
@@ -2924,13 +3755,16 @@
         <v>33</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H57" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2941,7 +3775,7 @@
         <v>33</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>21</v>
@@ -2955,10 +3789,10 @@
         <v>33</v>
       </c>
       <c r="D59" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>21</v>
@@ -2972,10 +3806,10 @@
         <v>33</v>
       </c>
       <c r="D60" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>22</v>
@@ -2989,10 +3823,10 @@
         <v>33</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>21</v>
@@ -3006,10 +3840,10 @@
         <v>33</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>21</v>
@@ -3023,10 +3857,10 @@
         <v>33</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>22</v>
@@ -3040,16 +3874,16 @@
         <v>33</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -3057,19 +3891,22 @@
         <v>33</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H65" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H65" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -3077,13 +3914,13 @@
         <v>33</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -3091,13 +3928,13 @@
         <v>33</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -3105,13 +3942,13 @@
         <v>33</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -3119,13 +3956,13 @@
         <v>33</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -3133,13 +3970,13 @@
         <v>33</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -3147,13 +3984,13 @@
         <v>33</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -3161,119 +3998,122 @@
         <v>33</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H72" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="I72" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>19</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>19</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>19</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>19</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>19</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>19</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>19</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>21</v>
@@ -3284,19 +4124,19 @@
         <v>19</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H81" t="s">
-        <v>56</v>
-      </c>
-      <c r="I81" s="9" t="s">
-        <v>40</v>
+        <v>54</v>
+      </c>
+      <c r="I81" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3304,18 +4144,18 @@
         <v>19</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H82" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="I82" s="9" t="s">
+      <c r="H82" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I82" s="8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3324,10 +4164,10 @@
         <v>19</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>21</v>
@@ -3338,10 +4178,10 @@
         <v>19</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>22</v>
@@ -3352,10 +4192,10 @@
         <v>19</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>24</v>
@@ -3366,10 +4206,10 @@
         <v>19</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>21</v>
@@ -3380,10 +4220,10 @@
         <v>19</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>25</v>
@@ -3394,10 +4234,10 @@
         <v>19</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>21</v>
@@ -3408,19 +4248,19 @@
         <v>19</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H89" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="I89" s="9" t="s">
-        <v>40</v>
+      <c r="H89" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I89" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3428,10 +4268,10 @@
         <v>19</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>21</v>
@@ -3442,10 +4282,10 @@
         <v>19</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>25</v>
@@ -3456,10 +4296,10 @@
         <v>19</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>21</v>
@@ -3470,10 +4310,10 @@
         <v>19</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>24</v>
@@ -3484,19 +4324,19 @@
         <v>19</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H94" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -3504,13 +4344,13 @@
         <v>19</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>21</v>
@@ -3521,13 +4361,13 @@
         <v>19</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>25</v>
@@ -3538,13 +4378,13 @@
         <v>19</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>21</v>
@@ -3555,13 +4395,13 @@
         <v>19</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>24</v>
@@ -3572,13 +4412,13 @@
         <v>19</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>21</v>
@@ -3589,22 +4429,22 @@
         <v>19</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I100" s="9" t="s">
-        <v>40</v>
+        <v>61</v>
+      </c>
+      <c r="I100" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -3612,13 +4452,13 @@
         <v>19</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D101" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>21</v>
@@ -3629,13 +4469,13 @@
         <v>19</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D102" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>25</v>
@@ -3646,13 +4486,13 @@
         <v>19</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D103" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F103" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>21</v>
@@ -3663,13 +4503,13 @@
         <v>19</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G104" s="3" t="s">
         <v>21</v>
@@ -3680,13 +4520,13 @@
         <v>19</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>22</v>
@@ -3697,13 +4537,13 @@
         <v>19</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>21</v>
@@ -3714,13 +4554,13 @@
         <v>19</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>25</v>
@@ -3731,13 +4571,13 @@
         <v>19</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>21</v>
@@ -3748,10 +4588,10 @@
         <v>19</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>21</v>
@@ -3762,10 +4602,10 @@
         <v>19</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>25</v>
@@ -3776,10 +4616,10 @@
         <v>19</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>21</v>
@@ -3790,255 +4630,258 @@
         <v>19</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>19</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>19</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>19</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>19</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H116" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H116" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I116" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>19</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>19</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>19</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>19</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>19</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>19</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>19</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>19</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>19</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>19</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G126" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>19</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G127" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>19</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G128" s="3" t="s">
         <v>22</v>
@@ -4049,13 +4892,13 @@
         <v>19</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G129" s="3" t="s">
         <v>21</v>
@@ -4066,13 +4909,13 @@
         <v>19</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G130" s="3" t="s">
         <v>25</v>
@@ -4083,13 +4926,13 @@
         <v>19</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>21</v>
@@ -4100,13 +4943,13 @@
         <v>19</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>22</v>
@@ -4117,22 +4960,22 @@
         <v>19</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I133" s="9" t="s">
-        <v>40</v>
+        <v>65</v>
+      </c>
+      <c r="I133" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4140,10 +4983,10 @@
         <v>19</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>21</v>
@@ -4154,10 +4997,10 @@
         <v>19</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>25</v>
@@ -4168,10 +5011,10 @@
         <v>19</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>21</v>
@@ -4182,10 +5025,10 @@
         <v>19</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>22</v>
@@ -4196,10 +5039,10 @@
         <v>19</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>21</v>
@@ -4210,10 +5053,10 @@
         <v>19</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>25</v>
@@ -4224,10 +5067,10 @@
         <v>19</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>21</v>
@@ -4238,10 +5081,10 @@
         <v>19</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>25</v>
@@ -4252,10 +5095,10 @@
         <v>19</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>21</v>
@@ -4266,19 +5109,19 @@
         <v>19</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H143" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I143" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4286,10 +5129,10 @@
         <v>19</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>21</v>
@@ -4300,10 +5143,10 @@
         <v>19</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>25</v>
@@ -4314,10 +5157,10 @@
         <v>19</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>21</v>
@@ -4328,10 +5171,10 @@
         <v>19</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>24</v>
@@ -4342,10 +5185,10 @@
         <v>19</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>21</v>
@@ -4356,10 +5199,10 @@
         <v>19</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>25</v>
@@ -4370,10 +5213,10 @@
         <v>19</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>21</v>
@@ -4384,19 +5227,19 @@
         <v>19</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H151" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I151" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4404,19 +5247,19 @@
         <v>19</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H152" s="18" t="s">
-        <v>75</v>
+      <c r="H152" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="I152" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -4424,10 +5267,10 @@
         <v>19</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>21</v>
@@ -4438,10 +5281,10 @@
         <v>19</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>22</v>
@@ -4452,10 +5295,10 @@
         <v>19</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>21</v>
@@ -4466,10 +5309,10 @@
         <v>19</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>25</v>
@@ -4480,235 +5323,262 @@
         <v>19</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="H157" s="4"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>19</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="H158" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I158" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>19</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="H159" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I159" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>19</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="H160" s="4"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>19</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="H161" s="4"/>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>19</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="H162" s="4"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>19</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H163" s="4"/>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>19</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="H164" s="4"/>
     </row>
     <row r="165" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>19</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="H165" s="4"/>
     </row>
     <row r="166" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>19</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H166" s="4"/>
     </row>
     <row r="167" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>19</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="H167" s="4"/>
     </row>
     <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>19</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="H168" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I168" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>19</v>
       </c>
-      <c r="B169" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C169" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="H169" s="20" t="s">
-        <v>96</v>
+      <c r="B169" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C169" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H169" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="I169" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>19</v>
       </c>
-      <c r="B170" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C170" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="H170" s="20" t="s">
-        <v>95</v>
+      <c r="B170" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C170" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H170" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="I170" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>19</v>
       </c>
-      <c r="B171" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C171" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="H171" s="20" t="s">
-        <v>99</v>
+      <c r="B171" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C171" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H171" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="I171" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>19</v>
       </c>
-      <c r="B172" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H172" s="21" t="s">
-        <v>85</v>
+      <c r="B172" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C172" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="H172" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="I172" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -4716,16 +5586,16 @@
         <v>19</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I173" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -4733,16 +5603,16 @@
         <v>19</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I174" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -4758,11 +5628,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A28" sqref="A3:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4772,246 +5642,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>40</v>
+      <c r="B4" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>40</v>
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>40</v>
+      <c r="A11" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>40</v>
+      <c r="B14" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>40</v>
+      <c r="A17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:B163">
-    <sortCondition ref="B2:B163"/>
+  <sortState ref="A2:B27">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Grado 11 - guion 01  Esqueleto y Correcc estilo ok
Ufff, cotejado el esqueleto con los cambios de estilo, había olvidado
ese detalle.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/esqueletoGuion - CS_11_01_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion01/esqueletoGuion - CS_11_01_CO.xlsx
@@ -326,9 +326,6 @@
     <t>Conflictos globales contemporáneos</t>
   </si>
   <si>
-    <t>El siglo XXI o la pugna por encontrar un lugar en el nuevo orden</t>
-  </si>
-  <si>
     <t>texto</t>
   </si>
   <si>
@@ -347,27 +344,18 @@
     <t>profundiza</t>
   </si>
   <si>
-    <t>Geopolítica: el planeta como tablero de juego</t>
-  </si>
-  <si>
     <t>practica</t>
   </si>
   <si>
     <t>La hegemonía estadounidense y la guerra contra el terrorismo</t>
   </si>
   <si>
-    <t>Reconfiguración continental y las regiones emergenes del mundo: Asia Pacífico y Eurasia</t>
-  </si>
-  <si>
     <t>Asia Pacífico</t>
   </si>
   <si>
     <t>Eurasia</t>
   </si>
   <si>
-    <t>Claves para comprender los conflictos del siglo XXI</t>
-  </si>
-  <si>
     <t>REC20. El juego geopolítico global</t>
   </si>
   <si>
@@ -389,9 +377,6 @@
     <t>REC60. Compara los conflictos tradicionales del siglo XX con los conflictos del siglo XXI</t>
   </si>
   <si>
-    <t>Las trasformaciones de los conflictos bélicos en el tercer milenio</t>
-  </si>
-  <si>
     <t>Los conflictos como oportunidades para el cambio social</t>
   </si>
   <si>
@@ -419,15 +404,9 @@
     <t>REC80. Formas no violentas para la resolución de conflictos</t>
   </si>
   <si>
-    <t>Conflictos bélicos actuales en Eurasia</t>
-  </si>
-  <si>
     <t>El retorno de los nacionalismos en la Unión Europea en crisis económica</t>
   </si>
   <si>
-    <t>Nuevas formas de fascismo recorren el corazón de Europa</t>
-  </si>
-  <si>
     <t>REC110. Comprende los nacionalismos en la Europa de hoy</t>
   </si>
   <si>
@@ -446,27 +425,12 @@
     <t>Chechenia</t>
   </si>
   <si>
-    <t>La forma en que se representa a los musulmanes desde la cultura occidental</t>
-  </si>
-  <si>
     <t>REC150. Construye una cronología en torno al conflicto Rusia-Ucrania</t>
   </si>
   <si>
-    <t>Chiitas y sunitas: claves para comprender los conflictos en Medio Oriente</t>
-  </si>
-  <si>
-    <t>Chiitas</t>
-  </si>
-  <si>
-    <t>Sunitas</t>
-  </si>
-  <si>
     <t>REC170. Comprende los conflictos entre chiitas y sunitas</t>
   </si>
   <si>
-    <t>Afganistán: tierra fértil para el fundamentalismo talibán y de las milicias de Al-Qaeda</t>
-  </si>
-  <si>
     <t>REC180. Las rutas del gas y del petróleo en Asia Central</t>
   </si>
   <si>
@@ -485,9 +449,6 @@
     <t>¿Quién controla la cabeza de las mujeres? El conflicto por el uso femenino del velo islámico</t>
   </si>
   <si>
-    <t>Ejercitación, proyectos y competencias</t>
-  </si>
-  <si>
     <t>Practica</t>
   </si>
   <si>
@@ -591,6 +552,45 @@
   </si>
   <si>
     <t>Una mirada panorámica a los conflictos globales escenificados en Europa y en Asia, identificando sus actores, los elementos y relaciones que implican desde la geopolítica</t>
+  </si>
+  <si>
+    <t>El siglo XXI o la pugna por encontrar un lugar en el Nuevo Orden Mundial</t>
+  </si>
+  <si>
+    <t>La geopolítica: el planeta como tablero de juego</t>
+  </si>
+  <si>
+    <t>La reconfiguración continental y las regiones emergenes del mundo: Asia Pacífico y Eurasia</t>
+  </si>
+  <si>
+    <t>Las claves para comprender los conflictos del siglo XXI</t>
+  </si>
+  <si>
+    <t>Las transformaciones de los conflictos bélicos en el tercer milenio</t>
+  </si>
+  <si>
+    <t>Los conflictos bélicos actuales en Eurasia</t>
+  </si>
+  <si>
+    <t>Las nuevas formas de fascismo recorren el corazón de Europa</t>
+  </si>
+  <si>
+    <t>La representación de los musulmanes desde la cultura occidental</t>
+  </si>
+  <si>
+    <t>Los chiitas y los sunitas: claves para comprender los conflictos en Medio Oriente</t>
+  </si>
+  <si>
+    <t>Los chiitas</t>
+  </si>
+  <si>
+    <t>Los sunitas</t>
+  </si>
+  <si>
+    <t>Afganistán: tierra fértil para el fundamentalismo talibán y las milicias de Al Qaeda</t>
+  </si>
+  <si>
+    <t>Consolidación</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1879,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -1887,7 +1887,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1895,7 +1895,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1967,19 +1967,19 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -1993,19 +1993,19 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -2013,42 +2013,42 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F4">
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="F5">
         <v>20</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2126,10 +2126,10 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2137,10 +2137,10 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2159,10 +2159,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -2170,10 +2170,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -2181,10 +2181,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -2192,10 +2192,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -2203,10 +2203,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>11</v>
@@ -2214,10 +2214,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>12</v>
@@ -2225,10 +2225,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>13</v>
@@ -2236,10 +2236,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>14</v>
@@ -2247,10 +2247,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C14">
         <v>15</v>
@@ -2258,10 +2258,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>17</v>
@@ -2269,10 +2269,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>18</v>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>19</v>
@@ -2291,10 +2291,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C18">
         <v>21</v>
@@ -2302,10 +2302,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19">
         <v>22</v>
@@ -2313,10 +2313,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C20">
         <v>23</v>
@@ -2324,10 +2324,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>24</v>
@@ -2335,10 +2335,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C22">
         <v>25</v>
@@ -2346,10 +2346,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C23">
         <v>26</v>
@@ -2357,10 +2357,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C24">
         <v>27</v>
@@ -2368,10 +2368,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C25">
         <v>28</v>
@@ -2379,10 +2379,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C26">
         <v>29</v>
@@ -2437,10 +2437,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2448,10 +2448,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2459,10 +2459,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2470,10 +2470,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2481,10 +2481,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2492,10 +2492,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2503,10 +2503,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2514,10 +2514,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2525,10 +2525,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2536,10 +2536,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2547,10 +2547,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2558,10 +2558,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2569,10 +2569,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2580,10 +2580,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2591,10 +2591,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2602,10 +2602,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2613,10 +2613,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2624,10 +2624,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2635,10 +2635,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2646,10 +2646,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2657,10 +2657,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2668,10 +2668,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2679,10 +2679,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2690,10 +2690,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2701,10 +2701,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2712,10 +2712,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2723,10 +2723,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2734,10 +2734,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2745,10 +2745,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2771,9 +2771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H169" sqref="H169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2823,10 +2823,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -2839,10 +2839,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2855,10 +2855,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -2871,10 +2871,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -2887,10 +2887,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -2903,14 +2903,14 @@
         <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -2921,14 +2921,14 @@
         <v>19</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -2939,14 +2939,14 @@
         <v>19</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -2957,14 +2957,14 @@
         <v>19</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -2975,14 +2975,14 @@
         <v>19</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -2993,14 +2993,14 @@
         <v>19</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -3011,22 +3011,22 @@
         <v>19</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3034,14 +3034,14 @@
         <v>19</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -3052,14 +3052,14 @@
         <v>19</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
@@ -3070,14 +3070,14 @@
         <v>19</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -3088,14 +3088,14 @@
         <v>19</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -3106,22 +3106,22 @@
         <v>19</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="8" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3129,14 +3129,14 @@
         <v>19</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -3147,14 +3147,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
@@ -3165,14 +3165,14 @@
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
@@ -3183,14 +3183,14 @@
         <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
@@ -3201,14 +3201,14 @@
         <v>19</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
@@ -3219,14 +3219,14 @@
         <v>19</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
@@ -3237,14 +3237,14 @@
         <v>19</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -3255,13 +3255,13 @@
         <v>19</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3269,19 +3269,19 @@
         <v>19</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3289,13 +3289,13 @@
         <v>19</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3303,16 +3303,16 @@
         <v>19</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3320,16 +3320,16 @@
         <v>19</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3337,16 +3337,16 @@
         <v>19</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3354,16 +3354,16 @@
         <v>19</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3371,16 +3371,16 @@
         <v>19</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3388,16 +3388,16 @@
         <v>19</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3405,16 +3405,16 @@
         <v>19</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3422,16 +3422,16 @@
         <v>19</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3439,16 +3439,16 @@
         <v>19</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3456,16 +3456,16 @@
         <v>19</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3473,16 +3473,16 @@
         <v>19</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3490,22 +3490,22 @@
         <v>19</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="I40" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3513,22 +3513,22 @@
         <v>19</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3536,10 +3536,10 @@
         <v>19</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3547,16 +3547,16 @@
         <v>19</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H43" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3564,13 +3564,13 @@
         <v>19</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3578,13 +3578,13 @@
         <v>19</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3592,13 +3592,13 @@
         <v>19</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3606,13 +3606,13 @@
         <v>19</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3620,13 +3620,13 @@
         <v>19</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3634,13 +3634,13 @@
         <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3648,13 +3648,13 @@
         <v>19</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3662,19 +3662,19 @@
         <v>19</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H51" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3682,13 +3682,13 @@
         <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3696,13 +3696,13 @@
         <v>19</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3710,13 +3710,13 @@
         <v>19</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3724,13 +3724,13 @@
         <v>19</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3738,13 +3738,13 @@
         <v>19</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3752,19 +3752,19 @@
         <v>19</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H57" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3772,13 +3772,13 @@
         <v>19</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3786,16 +3786,16 @@
         <v>19</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3803,16 +3803,16 @@
         <v>19</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3820,16 +3820,16 @@
         <v>19</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3837,16 +3837,16 @@
         <v>19</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3854,16 +3854,16 @@
         <v>19</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3871,16 +3871,16 @@
         <v>19</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3888,22 +3888,22 @@
         <v>19</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3911,13 +3911,13 @@
         <v>19</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3925,13 +3925,13 @@
         <v>19</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3939,13 +3939,13 @@
         <v>19</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3953,13 +3953,13 @@
         <v>19</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3967,13 +3967,13 @@
         <v>19</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3981,13 +3981,13 @@
         <v>19</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3995,19 +3995,19 @@
         <v>19</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H72" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -4015,10 +4015,10 @@
         <v>19</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4026,13 +4026,13 @@
         <v>19</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -4040,13 +4040,13 @@
         <v>19</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -4054,13 +4054,13 @@
         <v>19</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -4068,13 +4068,13 @@
         <v>19</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -4082,13 +4082,13 @@
         <v>19</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -4096,13 +4096,13 @@
         <v>19</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -4110,13 +4110,13 @@
         <v>19</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -4124,19 +4124,19 @@
         <v>19</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H81" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -4144,19 +4144,19 @@
         <v>19</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="I82" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -4164,13 +4164,13 @@
         <v>19</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -4178,13 +4178,13 @@
         <v>19</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -4192,13 +4192,13 @@
         <v>19</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -4206,13 +4206,13 @@
         <v>19</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -4220,13 +4220,13 @@
         <v>19</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -4234,13 +4234,13 @@
         <v>19</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -4248,19 +4248,19 @@
         <v>19</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -4268,13 +4268,13 @@
         <v>19</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -4282,13 +4282,13 @@
         <v>19</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -4296,13 +4296,13 @@
         <v>19</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4310,13 +4310,13 @@
         <v>19</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4324,19 +4324,19 @@
         <v>19</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H94" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4344,16 +4344,16 @@
         <v>19</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4361,16 +4361,16 @@
         <v>19</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4378,16 +4378,16 @@
         <v>19</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4395,16 +4395,16 @@
         <v>19</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4412,16 +4412,16 @@
         <v>19</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4429,22 +4429,22 @@
         <v>19</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4452,16 +4452,16 @@
         <v>19</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="G101" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4469,16 +4469,16 @@
         <v>19</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="G102" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4486,16 +4486,16 @@
         <v>19</v>
       </c>
       <c r="B103" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F103" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="G103" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4503,16 +4503,16 @@
         <v>19</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4520,16 +4520,16 @@
         <v>19</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4537,16 +4537,16 @@
         <v>19</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4554,16 +4554,16 @@
         <v>19</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4571,134 +4571,134 @@
         <v>19</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>19</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>19</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E110" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>19</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>19</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>19</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>19</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>19</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>19</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>19</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>19</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>19</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>19</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>19</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="H116" s="4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4706,13 +4706,13 @@
         <v>19</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4720,13 +4720,13 @@
         <v>19</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4734,13 +4734,13 @@
         <v>19</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4748,13 +4748,13 @@
         <v>19</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4762,13 +4762,13 @@
         <v>19</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4776,13 +4776,13 @@
         <v>19</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4790,16 +4790,16 @@
         <v>19</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4807,16 +4807,16 @@
         <v>19</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4824,16 +4824,16 @@
         <v>19</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4841,16 +4841,16 @@
         <v>19</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4858,16 +4858,16 @@
         <v>19</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4875,16 +4875,16 @@
         <v>19</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4892,16 +4892,16 @@
         <v>19</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4909,16 +4909,16 @@
         <v>19</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4926,16 +4926,16 @@
         <v>19</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4943,16 +4943,16 @@
         <v>19</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4960,22 +4960,22 @@
         <v>19</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="I133" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4983,13 +4983,13 @@
         <v>19</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4997,13 +4997,13 @@
         <v>19</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5011,13 +5011,13 @@
         <v>19</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5025,13 +5025,13 @@
         <v>19</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5039,13 +5039,13 @@
         <v>19</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5053,13 +5053,13 @@
         <v>19</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5067,13 +5067,13 @@
         <v>19</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5081,13 +5081,13 @@
         <v>19</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5095,13 +5095,13 @@
         <v>19</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5109,19 +5109,19 @@
         <v>19</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H143" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="I143" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5129,13 +5129,13 @@
         <v>19</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5143,13 +5143,13 @@
         <v>19</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5157,13 +5157,13 @@
         <v>19</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5171,13 +5171,13 @@
         <v>19</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5185,13 +5185,13 @@
         <v>19</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5199,13 +5199,13 @@
         <v>19</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5213,13 +5213,13 @@
         <v>19</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5227,19 +5227,19 @@
         <v>19</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H151" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="I151" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5247,19 +5247,19 @@
         <v>19</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H152" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="I152" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -5267,13 +5267,13 @@
         <v>19</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -5281,13 +5281,13 @@
         <v>19</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -5295,13 +5295,13 @@
         <v>19</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -5309,13 +5309,13 @@
         <v>19</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -5323,13 +5323,13 @@
         <v>19</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H157" s="4"/>
     </row>
@@ -5338,19 +5338,19 @@
         <v>19</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H158" s="4" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="I158" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -5358,19 +5358,19 @@
         <v>19</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H159" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="I159" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -5378,13 +5378,13 @@
         <v>19</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H160" s="4"/>
     </row>
@@ -5393,13 +5393,13 @@
         <v>19</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H161" s="4"/>
     </row>
@@ -5408,13 +5408,13 @@
         <v>19</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H162" s="4"/>
     </row>
@@ -5423,13 +5423,13 @@
         <v>19</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H163" s="4"/>
     </row>
@@ -5438,13 +5438,13 @@
         <v>19</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H164" s="4"/>
     </row>
@@ -5453,13 +5453,13 @@
         <v>19</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H165" s="4"/>
     </row>
@@ -5468,13 +5468,13 @@
         <v>19</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H166" s="4"/>
     </row>
@@ -5483,13 +5483,13 @@
         <v>19</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H167" s="4"/>
     </row>
@@ -5498,19 +5498,19 @@
         <v>19</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H168" s="4" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="I168" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -5518,16 +5518,16 @@
         <v>19</v>
       </c>
       <c r="B169" s="17" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C169" s="17" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H169" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="I169" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -5535,16 +5535,16 @@
         <v>19</v>
       </c>
       <c r="B170" s="17" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C170" s="17" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H170" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="I170" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -5552,16 +5552,16 @@
         <v>19</v>
       </c>
       <c r="B171" s="17" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C171" s="17" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H171" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I171" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -5569,16 +5569,16 @@
         <v>19</v>
       </c>
       <c r="B172" s="17" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C172" s="17" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="H172" s="16" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="I172" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -5586,16 +5586,16 @@
         <v>19</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="I173" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -5603,16 +5603,16 @@
         <v>19</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I174" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -5651,210 +5651,210 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>